<commit_message>
Updated epi_codec_video.py for better memory utilization and added benchmark results of the last two datasets in result.xlsx
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\losor\Desktop\coding\Compressione_Dati\lfi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD286181-4AE1-4703-84A4-C77EDC5DB645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922ABA93-6753-45E3-9256-72369140D634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bikes" sheetId="1" r:id="rId1"/>
     <sheet name="Danger_de_Mort" sheetId="3" r:id="rId2"/>
     <sheet name="greek" sheetId="4" r:id="rId3"/>
     <sheet name="sideboard" sheetId="5" r:id="rId4"/>
+    <sheet name="tarot" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
   <si>
     <t>Codec</t>
   </si>
@@ -166,6 +167,57 @@
   </si>
   <si>
     <t>392.61:1</t>
+  </si>
+  <si>
+    <t>85.66:1</t>
+  </si>
+  <si>
+    <t>26.12:1</t>
+  </si>
+  <si>
+    <t>19.93:1</t>
+  </si>
+  <si>
+    <t>24.65:1</t>
+  </si>
+  <si>
+    <t>91.87:1</t>
+  </si>
+  <si>
+    <t>65.56:1</t>
+  </si>
+  <si>
+    <t>110.09:1</t>
+  </si>
+  <si>
+    <t>Grid: 17 x 17</t>
+  </si>
+  <si>
+    <t>Img Size: 1024 x 1024</t>
+  </si>
+  <si>
+    <t>Orig. Size (MB): 1734.00 MB</t>
+  </si>
+  <si>
+    <t>150.56:1</t>
+  </si>
+  <si>
+    <t>31.39:1</t>
+  </si>
+  <si>
+    <t>30.30:1</t>
+  </si>
+  <si>
+    <t>37.03:1</t>
+  </si>
+  <si>
+    <t>964.52:1</t>
+  </si>
+  <si>
+    <t>366.82:1</t>
+  </si>
+  <si>
+    <t>380.96:1</t>
   </si>
 </sst>
 </file>
@@ -1550,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77941275-37C3-4181-8BE8-1A7A129D8D51}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1611,43 +1663,267 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="B2" s="4">
+        <v>1.42</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.98829999999999996</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.56030000000000002</v>
+      </c>
+      <c r="F2" s="4">
+        <v>700</v>
+      </c>
+      <c r="G2" s="4">
+        <v>34.79</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.97428099999999995</v>
+      </c>
+      <c r="J2" s="4">
+        <v>3.1229999999999999E-3</v>
+      </c>
+      <c r="K2" s="4">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4">
+        <v>3.7</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="B3">
+        <v>1.32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.98909999999999998</v>
+      </c>
+      <c r="E3">
+        <v>0.52249999999999996</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>34.36</v>
+      </c>
+      <c r="H3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I3">
+        <v>0.97402299999999997</v>
+      </c>
+      <c r="J3">
+        <v>2.8479999999999998E-3</v>
+      </c>
+      <c r="K3">
+        <v>2.7</v>
+      </c>
+      <c r="L3">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="4" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="B4" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.9909</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.436</v>
+      </c>
+      <c r="F4" s="4">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4">
+        <v>34.549999999999997</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.97442200000000001</v>
+      </c>
+      <c r="J4" s="4">
+        <v>8.2299999999999995E-4</v>
+      </c>
+      <c r="K4" s="4">
+        <v>11.1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2.4</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="B5">
+        <v>1.85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.98470000000000002</v>
+      </c>
+      <c r="E5">
+        <v>0.73209999999999997</v>
+      </c>
+      <c r="F5">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>34.53</v>
+      </c>
+      <c r="H5">
+        <v>0.54</v>
+      </c>
+      <c r="I5">
+        <v>0.97411300000000001</v>
+      </c>
+      <c r="J5">
+        <v>2.7420000000000001E-3</v>
+      </c>
+      <c r="K5">
+        <v>7.1</v>
+      </c>
+      <c r="L5">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="B6" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.94979999999999998</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.4081000000000001</v>
+      </c>
+      <c r="F6" s="4">
+        <v>13</v>
+      </c>
+      <c r="G6" s="4">
+        <v>34.14</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1.02</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.97418000000000005</v>
+      </c>
+      <c r="J6" s="4">
+        <v>5.267E-3</v>
+      </c>
+      <c r="K6" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1.29</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="B7">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.9617</v>
+      </c>
+      <c r="E7">
+        <v>1.8379000000000001</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>34.619999999999997</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.97447300000000003</v>
+      </c>
+      <c r="J7">
+        <v>4.9779999999999998E-3</v>
+      </c>
+      <c r="K7">
+        <v>17.32</v>
+      </c>
+      <c r="L7">
+        <v>1.19</v>
+      </c>
     </row>
     <row r="8" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="B8" s="4">
+        <v>4.93</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.95940000000000003</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.9476</v>
+      </c>
+      <c r="F8" s="4">
+        <v>14</v>
+      </c>
+      <c r="G8" s="4">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.97397800000000001</v>
+      </c>
+      <c r="J8" s="4">
+        <v>5.0179999999999999E-3</v>
+      </c>
+      <c r="K8" s="4">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1.1200000000000001</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -1662,6 +1938,353 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D36A94A-703B-47EA-A9F9-520EE57A549D}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" customWidth="1"/>
+    <col min="12" max="12" width="15.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.99339999999999995</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.31879999999999997</v>
+      </c>
+      <c r="F2" s="4">
+        <v>700</v>
+      </c>
+      <c r="G2" s="4">
+        <v>36.99</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.97370999999999996</v>
+      </c>
+      <c r="J2" s="4">
+        <v>2.0509999999999999E-3</v>
+      </c>
+      <c r="K2" s="4">
+        <v>316.5</v>
+      </c>
+      <c r="L2" s="4">
+        <v>48.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>4.55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.99739999999999995</v>
+      </c>
+      <c r="E3">
+        <v>0.126</v>
+      </c>
+      <c r="F3">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>36.32</v>
+      </c>
+      <c r="H3">
+        <v>0.84</v>
+      </c>
+      <c r="I3">
+        <v>0.97431699999999999</v>
+      </c>
+      <c r="J3">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="K3">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="L3">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.999</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>31</v>
+      </c>
+      <c r="G4" s="4">
+        <v>35.97</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.97367599999999999</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1.049E-3</v>
+      </c>
+      <c r="K4" s="4">
+        <v>54.4</v>
+      </c>
+      <c r="L4" s="4">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.99729999999999996</v>
+      </c>
+      <c r="E5">
+        <v>0.13089999999999999</v>
+      </c>
+      <c r="F5">
+        <v>32</v>
+      </c>
+      <c r="G5">
+        <v>36.19</v>
+      </c>
+      <c r="H5">
+        <v>0.85</v>
+      </c>
+      <c r="I5">
+        <v>0.97333999999999998</v>
+      </c>
+      <c r="J5">
+        <v>2.4710000000000001E-3</v>
+      </c>
+      <c r="K5">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="L5">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="4">
+        <v>57.23</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.5841000000000001</v>
+      </c>
+      <c r="F6" s="4">
+        <v>13</v>
+      </c>
+      <c r="G6" s="4">
+        <v>36.57</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.97402</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.8709999999999995E-3</v>
+      </c>
+      <c r="K6" s="4">
+        <v>22.95</v>
+      </c>
+      <c r="L6" s="4">
+        <v>9.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>46.82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="E7">
+        <v>1.2962</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>36.86</v>
+      </c>
+      <c r="H7">
+        <v>2.36</v>
+      </c>
+      <c r="I7">
+        <v>0.97379199999999999</v>
+      </c>
+      <c r="J7">
+        <v>7.4440000000000001E-3</v>
+      </c>
+      <c r="K7">
+        <v>130</v>
+      </c>
+      <c r="L7">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4">
+        <v>55.23</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.96809999999999996</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.5289999999999999</v>
+      </c>
+      <c r="F8" s="4">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4">
+        <v>36.96</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2.41</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.97373600000000005</v>
+      </c>
+      <c r="J8" s="4">
+        <v>7.6270000000000001E-3</v>
+      </c>
+      <c r="K8" s="4">
+        <v>65</v>
+      </c>
+      <c r="L8" s="4">
+        <v>9.56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>